<commit_message>
mise à jour des fonctionnalités
</commit_message>
<xml_diff>
--- a/Spécifications/Cadrage_Fonctionnel_FVX.xlsx
+++ b/Spécifications/Cadrage_Fonctionnel_FVX.xlsx
@@ -28,7 +28,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
   <si>
     <t xml:space="preserve">Personne interviewée</t>
   </si>
@@ -328,79 +328,79 @@
     <t xml:space="preserve">Priorité</t>
   </si>
   <si>
-    <t xml:space="preserve">Chiffrage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statut</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gérer un admin</t>
   </si>
   <si>
-    <t xml:space="preserve">En tant qu’admin, je veux pouvoir récupérer une donnée dans le but de vérifier que les informations sont correctes</t>
+    <t xml:space="preserve">En tant qu’admin je veux pouvoir me connecter dans le but d’avoir accès à un espace privilégié.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’admin doit avoir un login et un mot de passe qui doivent être enregistrés dans la base de données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir voir les demandes pour devenir superviseur dans le but d’accepter ou de décliner un nouveau superviseur.</t>
   </si>
   <si>
     <t xml:space="preserve">L’admin doit être connecté à l’application</t>
   </si>
   <si>
+    <t xml:space="preserve">P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir ajouter une donnée pour une salle dans le but de collecter des informations pour entraîner le modèle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir créer une salle dans le but d’en ajouter une nouvelle.</t>
+  </si>
+  <si>
     <t xml:space="preserve">P3</t>
   </si>
   <si>
-    <t xml:space="preserve">EN COURS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En tant qu'admin, je veux pouvoir supprimer une donnée dans le but de mettre à jour les informations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NON INITIE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En tant qu’admin, je veux pouvoir me connecter dans le but d’avoir accès à un espace privilégié</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’admin doit avoir un login et un mot de passe qui doivent être enregistrés dans la base de données</t>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir créer un étage dans le but d’en ajouter un nouveau.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir créer un bâtiment dans le but d’en ajouter un nouveau.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir créer un campus dans le but d’en ajouter un nouveau.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir visualiser les données d’une salle dans le but de vérifier que les informations sont correctes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin, je veux pouvoir supprimer les données d’une salle dans le but de mettre à jour les informations.</t>
   </si>
   <si>
     <t xml:space="preserve">Gérer un superviseur</t>
   </si>
   <si>
-    <t xml:space="preserve">En tant que superviseur, je veux ajouter une donnée pour une salle dans le but de collecter des informations pour entraîner le modèle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le superviseur doit avoir un login et un mot de passe qui doivent être enregistrés dans la base de données et la salle doit être existante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En tant que superviseur, je veux pouvoir me connecter dans le but d’avoir accès à un espace privilégié</t>
+    <t xml:space="preserve">En tant que superviseur je veux pouvoir me connecter dans le but d’avoir accès à un espace privilégié.</t>
   </si>
   <si>
     <t xml:space="preserve">Le superviseur doit avoir un login et un mot de passe qui doivent être enregistrés dans la base de données</t>
   </si>
   <si>
+    <t xml:space="preserve">En tant que superviseur, je veux pouvoir ajouter une donnée pour une salle dans le but de collecter des informations pour entraîner le modèle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le superviseur doit être connecté à l’application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant que superviseur, je veux pouvoir visualiser les données d’une salle dans le but de vérifier que les informations sont correctes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant que superviseur, je veux pouvoir supprimer les données d’une salle dans le but de mettre à jour les informations.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gérer un utilisateur</t>
   </si>
   <si>
-    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir me localiser pour connaître ma position dans un bâtiment</t>
+    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir me localiser pour connaître ma position dans un bâtiment.</t>
   </si>
   <si>
     <t xml:space="preserve">L’application possède un bouton qui permet de se localiser</t>
@@ -409,13 +409,19 @@
     <t xml:space="preserve">P0</t>
   </si>
   <si>
-    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir choisir le mode d’affichage dans le but d’avoir la vue souhaitée</t>
+    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir choisir le mode d’affichage dans le but d’avoir la vue souhaitée.</t>
   </si>
   <si>
     <t xml:space="preserve">L’application possède un bouton pour changer de mode d’affichage</t>
   </si>
   <si>
-    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir reporter un problème dans le but d’améliorer l’application</t>
+    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir devenir superviseur dans le but de collecter des données pour le modèle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’application possède un bouton pour devenir superviseur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir reporter un problème dans le but d’améliorer l’application.</t>
   </si>
   <si>
     <t xml:space="preserve">- Reporter un mauvais plan
@@ -424,12 +430,6 @@
   </si>
   <si>
     <t xml:space="preserve">L’application possède un bouton pour reporter un problème</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P3 = optionnel</t>
   </si>
   <si>
     <t xml:space="preserve">Description du risque</t>
@@ -538,12 +538,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
-        <bgColor rgb="FFDEEBF7"/>
+        <bgColor rgb="FFCDF1CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEEBF7"/>
+        <fgColor rgb="FFCDF1CE"/>
         <bgColor rgb="FFDDEBF7"/>
       </patternFill>
     </fill>
@@ -606,57 +606,77 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -667,10 +687,30 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -679,32 +719,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -759,8 +783,8 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFDEEBF7"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCDF1CE"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF9DC3E6"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -788,8 +812,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau134567891011121316" displayName="Tableau134567891011121316" ref="A1:M13" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:M13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau134567891011121316" displayName="Tableau134567891011121316" ref="A1:M22" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:M22"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Module"/>
     <tableColumn id="2" name="Cas Utilisation"/>
@@ -797,13 +821,13 @@
     <tableColumn id="4" name="Sous-fonctionnalités (si existante)"/>
     <tableColumn id="5" name="Règles de gestion (contraintes)"/>
     <tableColumn id="6" name="Priorité"/>
-    <tableColumn id="7" name="Chiffrage"/>
-    <tableColumn id="8" name="SP1"/>
-    <tableColumn id="9" name="SP2"/>
-    <tableColumn id="10" name="SP3"/>
-    <tableColumn id="11" name="SP4"/>
-    <tableColumn id="12" name="SP5"/>
-    <tableColumn id="13" name="Statut"/>
+    <tableColumn id="7" name=""/>
+    <tableColumn id="8" name=""/>
+    <tableColumn id="9" name=""/>
+    <tableColumn id="10" name=""/>
+    <tableColumn id="11" name=""/>
+    <tableColumn id="12" name=""/>
+    <tableColumn id="13" name=""/>
   </tableColumns>
 </table>
 </file>
@@ -854,21 +878,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.8097165991903"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="122.651821862348"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.2348178137652"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="123.720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.165991902834"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.4615384615385"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -892,7 +916,7 @@
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -934,7 +958,7 @@
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
@@ -1362,30 +1386,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="139.574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="82.3724696356275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="140.862348178138"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="83.0161943319838"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.4615384615385"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>67</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
@@ -1407,7 +1436,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1423,7 +1452,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1457,23 +1486,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.3805668016194"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="113.651821862348"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.2024291497976"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="114.724696356275"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="1" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.4615384615385"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
@@ -1492,176 +1522,178 @@
       <c r="F1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="28.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="F2" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
-      <c r="M2" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="13"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="13"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="12" t="s">
-        <v>98</v>
-      </c>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="13"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
-      <c r="B6" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="13"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="13"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
-      <c r="M7" s="12" t="s">
-        <v>98</v>
-      </c>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1670,173 +1702,460 @@
     </row>
     <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
-      <c r="B10" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
-      <c r="C11" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="19"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="20"/>
-      <c r="C12" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="19"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
-        <v>116</v>
-      </c>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="20"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="19"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="15"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C16" s="4"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="M16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="4"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="0"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="14"/>
-      <c r="H19" s="26"/>
-      <c r="M19" s="17"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="14"/>
-      <c r="H20" s="26"/>
-    </row>
-    <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M21" s="17"/>
-    </row>
-    <row r="22" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M22" s="17"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="22"/>
+      <c r="C21" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" customFormat="false" ht="55.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="0"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M23" s="17"/>
+      <c r="A23" s="0"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M24" s="17"/>
-    </row>
-    <row r="25" customFormat="false" ht="71.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M25" s="17"/>
+      <c r="A24" s="0"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="0"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M26" s="17"/>
+      <c r="A26" s="0"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M27" s="17"/>
-    </row>
-    <row r="28" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="0"/>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="27"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="27"/>
+    </row>
+    <row r="31" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="27"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="27"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
+      <c r="M33" s="27"/>
+    </row>
+    <row r="34" customFormat="false" ht="71.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="27"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+      <c r="M35" s="27"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+      <c r="J36" s="0"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+      <c r="M36" s="27"/>
+    </row>
+    <row r="37" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1865,16 +2184,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.4615384615385"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajout de nouvelles fonctionnalités attribuées à l'admin
</commit_message>
<xml_diff>
--- a/Spécifications/Cadrage_Fonctionnel_FVX.xlsx
+++ b/Spécifications/Cadrage_Fonctionnel_FVX.xlsx
@@ -28,7 +28,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B13" authorId="0">
+    <comment ref="B19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0">
+    <comment ref="B26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="129">
   <si>
     <t xml:space="preserve">Personne interviewée</t>
   </si>
@@ -378,6 +378,21 @@
     <t xml:space="preserve">En tant qu’admin, je veux pouvoir supprimer les données d’un superviseur dans le but de garder des données correctes.</t>
   </si>
   <si>
+    <t xml:space="preserve">En tant qu’admin je veux pouvoir supprimer le compte d’un superviseur dans le but d’avoir des superviseurs fiables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin je veux pouvoir supprimer un campus dans le but d’avoir de mettre à jour les données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin je veux pouvoir supprimer un bâtiment dans le but d’avoir de mettre à jour les données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin je veux pouvoir supprimer un étage dans le but d’avoir de mettre à jour les données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin je veux pouvoir supprimer une salle dans le but d’avoir de mettre à jour les données</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gérer un superviseur</t>
   </si>
   <si>
@@ -415,17 +430,17 @@
   </si>
   <si>
     <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir choisir le mode d’affichage dans le but d’avoir la vue souhaitée.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’application possède un bouton pour devenir superviseur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir devenir superviseur dans le but de collecter des données pour le modèle.</t>
   </si>
   <si>
     <t xml:space="preserve">- Reporter un mauvais plan
 - Reporter un dysfonctionnement de l’application
 - Reporter une mauvaise localisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’application possède un bouton pour devenir superviseur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’utilisateur, je veux pouvoir devenir superviseur dans le but de collecter des données pour le modèle.</t>
   </si>
   <si>
     <t xml:space="preserve">L’application possède un bouton pour reporter un problème</t>
@@ -653,6 +668,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -669,22 +688,22 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -693,24 +712,20 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -850,7 +865,7 @@
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="59.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.7"/>
@@ -1357,7 +1372,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.74"/>
@@ -1458,13 +1473,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.8"/>
@@ -1713,13 +1728,17 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="10" t="s">
+        <v>101</v>
+      </c>
       <c r="D12" s="11"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1728,15 +1747,17 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
-      <c r="B13" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="G13" s="12"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1745,18 +1766,16 @@
       <c r="L13" s="8"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
       <c r="B14" s="3"/>
       <c r="C14" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
         <v>103</v>
       </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="12" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="8"/>
@@ -1766,18 +1785,16 @@
       <c r="L14" s="8"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="3"/>
       <c r="C15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="8"/>
@@ -1787,18 +1804,16 @@
       <c r="L15" s="8"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
       <c r="B16" s="3"/>
       <c r="C16" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>87</v>
+      <c r="D16" s="11"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="8"/>
@@ -1808,20 +1823,14 @@
       <c r="L16" s="8"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D17" s="0"/>
-      <c r="E17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="14"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="0"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1831,12 +1840,12 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
-      <c r="B18" s="0"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="0"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="0"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1846,12 +1855,14 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="0"/>
+      <c r="B19" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="0"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="0"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1859,20 +1870,20 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" s="14"/>
+      <c r="F20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="12"/>
       <c r="H20" s="0"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -1880,21 +1891,21 @@
       <c r="L20" s="8"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="19"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1902,41 +1913,39 @@
       <c r="M21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D22" s="0"/>
-      <c r="E22" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="19"/>
+      <c r="E22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
-      <c r="B23" s="18"/>
+      <c r="B23" s="0"/>
       <c r="C23" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="D23" s="0"/>
+      <c r="E23" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="G23" s="15"/>
       <c r="H23" s="0"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -1946,15 +1955,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="17"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="19"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1963,12 +1970,12 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="0"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -1978,12 +1985,18 @@
     </row>
     <row r="26" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="B26" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" s="15"/>
       <c r="H26" s="0"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -1994,55 +2007,77 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
       <c r="B27" s="0"/>
-      <c r="C27" s="22"/>
+      <c r="C27" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="E27" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="15"/>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
       <c r="L27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="15"/>
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
       <c r="L28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="27"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="0"/>
       <c r="J29" s="0"/>
       <c r="K29" s="0"/>
       <c r="L29" s="0"/>
-      <c r="M29" s="17"/>
+      <c r="M29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="27"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="21"/>
       <c r="I30" s="0"/>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
@@ -2050,78 +2085,83 @@
     </row>
     <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
       <c r="L31" s="0"/>
-      <c r="M31" s="17"/>
+      <c r="M31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="0"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
       <c r="L32" s="0"/>
-      <c r="M32" s="17"/>
+      <c r="M32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="0"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="0"/>
-      <c r="F33" s="0"/>
-      <c r="G33" s="0"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
       <c r="L33" s="0"/>
-      <c r="M33" s="17"/>
+      <c r="M33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="0"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="0"/>
-      <c r="E34" s="0"/>
-      <c r="F34" s="0"/>
-      <c r="G34" s="0"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
       <c r="J34" s="0"/>
       <c r="K34" s="0"/>
       <c r="L34" s="0"/>
-      <c r="M34" s="17"/>
+      <c r="M34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="71.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
       <c r="B35" s="0"/>
+      <c r="C35" s="4"/>
       <c r="D35" s="0"/>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
-      <c r="G35" s="0"/>
+      <c r="G35" s="15"/>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
       <c r="J35" s="0"/>
       <c r="K35" s="0"/>
       <c r="L35" s="0"/>
-      <c r="M35" s="17"/>
+      <c r="M35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="0"/>
+      <c r="C36" s="4"/>
       <c r="D36" s="0"/>
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
@@ -2131,11 +2171,12 @@
       <c r="J36" s="0"/>
       <c r="K36" s="0"/>
       <c r="L36" s="0"/>
-      <c r="M36" s="17"/>
+      <c r="M36" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="0"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="0"/>
       <c r="E37" s="0"/>
       <c r="F37" s="0"/>
@@ -2145,10 +2186,48 @@
       <c r="J37" s="0"/>
       <c r="K37" s="0"/>
       <c r="L37" s="0"/>
-      <c r="M37" s="17"/>
-    </row>
-    <row r="38" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="M37" s="19"/>
+    </row>
+    <row r="38" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2175,7 +2254,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.78"/>
@@ -2183,23 +2262,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
ajout de la fonctionnalité de réinitialisation de la base de données
</commit_message>
<xml_diff>
--- a/Spécifications/Cadrage_Fonctionnel_FVX.xlsx
+++ b/Spécifications/Cadrage_Fonctionnel_FVX.xlsx
@@ -28,7 +28,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B19" authorId="0">
+    <comment ref="B20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0">
+    <comment ref="B28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="130">
   <si>
     <t xml:space="preserve">Personne interviewée</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t xml:space="preserve">En tant qu’admin je veux pouvoir supprimer une salle dans le but d’avoir de mettre à jour les données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant qu’admin je veux pouvoir réinitialiser la base de données dans le but d’enlever toutes les données si le modèle est mauvais</t>
   </si>
   <si>
     <t xml:space="preserve">Gérer un superviseur</t>
@@ -790,8 +793,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau134567891011121316" displayName="Tableau134567891011121316" ref="A1:M23" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:M23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau134567891011121316" displayName="Tableau134567891011121316" ref="A1:M24" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:M24"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Module"/>
     <tableColumn id="2" name="Cas Utilisation"/>
@@ -856,10 +859,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.0890688259109"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="125.866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.8421052631579"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.8380566801619"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="127.044534412955"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.4615384615385"/>
   </cols>
   <sheetData>
@@ -1365,9 +1368,9 @@
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="143.433198380567"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="84.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="144.716599190283"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="85.2672064777328"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.4615384615385"/>
   </cols>
@@ -1464,19 +1467,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.5182186234818"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="116.651821862348"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.2672064777328"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="117.724696356275"/>
     <col collapsed="false" hidden="false" max="12" min="6" style="1" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.4615384615385"/>
   </cols>
@@ -1825,13 +1828,19 @@
       <c r="L16" s="8"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="12"/>
+      <c r="E17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="G17" s="12"/>
       <c r="H17" s="0"/>
       <c r="I17" s="8"/>
@@ -1843,8 +1852,8 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="3"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -1857,13 +1866,11 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
-      <c r="B19" s="9" t="s">
-        <v>106</v>
-      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="0"/>
       <c r="I19" s="8"/>
@@ -1872,42 +1879,38 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>107</v>
       </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
       <c r="G20" s="12"/>
       <c r="H20" s="0"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="10"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="3"/>
       <c r="C21" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="H21" s="0"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1915,19 +1918,19 @@
       <c r="M21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="3"/>
       <c r="C22" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="0"/>
-      <c r="E22" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="15"/>
+      <c r="F22" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="12"/>
       <c r="H22" s="13"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1937,34 +1940,40 @@
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="10" t="s">
         <v>112</v>
       </c>
       <c r="D23" s="0"/>
       <c r="E23" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>87</v>
       </c>
       <c r="G23" s="15"/>
-      <c r="H23" s="0"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="0"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="10" t="s">
+        <v>113</v>
+      </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="14"/>
+      <c r="E24" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>87</v>
+      </c>
       <c r="G24" s="15"/>
-      <c r="H24" s="13"/>
+      <c r="H24" s="0"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1974,31 +1983,27 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="0"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="0"/>
-      <c r="E25" s="0"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="14"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="0"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
-      <c r="B26" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="0"/>
-      <c r="F26" s="14" t="s">
-        <v>114</v>
-      </c>
+      <c r="B26" s="0"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="14"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="0"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -2008,120 +2013,124 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
       <c r="B27" s="0"/>
-      <c r="C27" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="C27" s="16"/>
       <c r="D27" s="0"/>
-      <c r="E27" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>90</v>
-      </c>
+      <c r="E27" s="0"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="15"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
-      <c r="J27" s="0"/>
-      <c r="K27" s="0"/>
-      <c r="L27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="55.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>119</v>
-      </c>
+      <c r="B28" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="0"/>
       <c r="F28" s="14" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="0"/>
-      <c r="J28" s="0"/>
-      <c r="K28" s="0"/>
-      <c r="L28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="18"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="0"/>
       <c r="E29" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F29" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>90</v>
       </c>
       <c r="G29" s="15"/>
-      <c r="H29" s="21"/>
+      <c r="H29" s="0"/>
       <c r="I29" s="0"/>
       <c r="J29" s="0"/>
       <c r="K29" s="0"/>
       <c r="L29" s="0"/>
-      <c r="M29" s="19"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="55.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="18"/>
+      <c r="C30" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>119</v>
+      </c>
       <c r="E30" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="15"/>
+        <v>120</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>90</v>
+      </c>
       <c r="G30" s="15"/>
-      <c r="H30" s="21"/>
+      <c r="H30" s="0"/>
       <c r="I30" s="0"/>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
       <c r="L30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="18"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="15"/>
+      <c r="C31" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="G31" s="15"/>
-      <c r="H31" s="0"/>
+      <c r="H31" s="21"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
       <c r="L31" s="0"/>
       <c r="M31" s="19"/>
     </row>
-    <row r="32" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
-      <c r="B32" s="0"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="25"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19" t="s">
+        <v>124</v>
+      </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
-      <c r="H32" s="0"/>
+      <c r="H32" s="21"/>
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
       <c r="L32" s="0"/>
-      <c r="M32" s="19"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
+      <c r="B33" s="18"/>
       <c r="C33" s="23"/>
-      <c r="D33" s="0"/>
-      <c r="E33" s="26"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="0"/>
@@ -2131,12 +2140,12 @@
       <c r="L33" s="0"/>
       <c r="M33" s="19"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="0"/>
       <c r="C34" s="23"/>
       <c r="D34" s="0"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="25"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="0"/>
@@ -2146,13 +2155,13 @@
       <c r="L34" s="0"/>
       <c r="M34" s="19"/>
     </row>
-    <row r="35" customFormat="false" ht="71.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
       <c r="B35" s="0"/>
-      <c r="C35" s="4"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="0"/>
-      <c r="E35" s="0"/>
-      <c r="F35" s="0"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
@@ -2164,11 +2173,11 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="0"/>
-      <c r="C36" s="4"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
-      <c r="F36" s="0"/>
-      <c r="G36" s="0"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
       <c r="H36" s="0"/>
       <c r="I36" s="0"/>
       <c r="J36" s="0"/>
@@ -2176,14 +2185,14 @@
       <c r="L36" s="0"/>
       <c r="M36" s="19"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="71.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="0"/>
       <c r="C37" s="4"/>
       <c r="D37" s="0"/>
       <c r="E37" s="0"/>
       <c r="F37" s="0"/>
-      <c r="G37" s="0"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="0"/>
       <c r="I37" s="0"/>
       <c r="J37" s="0"/>
@@ -2191,8 +2200,38 @@
       <c r="L37" s="0"/>
       <c r="M37" s="19"/>
     </row>
-    <row r="38" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="J38" s="0"/>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
+      <c r="M38" s="19"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="M39" s="19"/>
+    </row>
+    <row r="40" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2221,30 +2260,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.4615384615385"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>